<commit_message>
Local Search 1 wersja
</commit_message>
<xml_diff>
--- a/program/dane.xlsx
+++ b/program/dane.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uzytkownik\Desktop\MIS\MIS\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDDD954-53AA-4C05-9F91-8AD961318421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E662E6-C514-461D-8D11-E69D130AEDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Capacity</t>
   </si>
@@ -39,30 +50,6 @@
     <t>Zapotrzebowanie</t>
   </si>
   <si>
-    <t>Kowalski</t>
-  </si>
-  <si>
-    <t>Nowak</t>
-  </si>
-  <si>
-    <t>Kajtek</t>
-  </si>
-  <si>
-    <t>bacan</t>
-  </si>
-  <si>
-    <t>Canvuil</t>
-  </si>
-  <si>
-    <t>Zoju</t>
-  </si>
-  <si>
-    <t>Donovan</t>
-  </si>
-  <si>
-    <t>Kasztan</t>
-  </si>
-  <si>
     <t>Czas Obslugi</t>
   </si>
   <si>
@@ -82,6 +69,12 @@
   </si>
   <si>
     <t>Poprzednik AND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">czas jazdy * koszt jazdy+koszt obsługi * czas obsługi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">czas całkowity </t>
   </si>
 </sst>
 </file>
@@ -399,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="F19" sqref="F19:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,59 +424,56 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10000</v>
+        <v>140</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+      <c r="H2">
         <v>8</v>
       </c>
-      <c r="G2">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>14</v>
-      </c>
       <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2">
         <v>5</v>
       </c>
     </row>
@@ -492,77 +482,167 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
         <v>14</v>
       </c>
-      <c r="G3">
-        <v>16</v>
-      </c>
       <c r="H3">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I3">
-        <v>213</v>
-      </c>
-      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
-        <v>7</v>
+      <c r="K3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>15</v>
       </c>
       <c r="H4">
-        <v>231</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>12</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5">
-        <v>1500</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="I5">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>17</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
+      <c r="I7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chyba dzialajacy w koncu programik
</commit_message>
<xml_diff>
--- a/program/dane.xlsx
+++ b/program/dane.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uzytkownik\Desktop\MIS\MIS\program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bilin\Desktop\magisterka s2\metody inżynierii systemów\projekt\MIS\program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9635E541-386C-409B-9241-30179709DE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD6CC26-BB02-476D-B643-A5C5683D7C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7035" yWindow="2970" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
         <v>140</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -568,7 +568,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E9">
         <v>3</v>

</xml_diff>